<commit_message>
Commit Add a data
</commit_message>
<xml_diff>
--- a/Rediness check list.xlsx
+++ b/Rediness check list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" tabRatio="721" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20740" windowHeight="11760" tabRatio="721" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Check List" sheetId="7" r:id="rId1"/>
     <sheet name="Scrum Tracking" sheetId="8" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
   <si>
     <t>Boonyavee</t>
   </si>
@@ -164,6 +164,12 @@
   <si>
     <t>- test the GD Code with JavaAdapter
 - Continue with real mechanism</t>
+  </si>
+  <si>
+    <t>MATI</t>
+  </si>
+  <si>
+    <t>TEST</t>
   </si>
 </sst>
 </file>
@@ -388,15 +394,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -420,6 +417,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="89">
@@ -825,83 +831,83 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="101.5703125" customWidth="1"/>
-    <col min="3" max="10" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.7109375" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" style="1" customWidth="1"/>
-    <col min="260" max="260" width="86.28515625" customWidth="1"/>
-    <col min="516" max="516" width="86.28515625" customWidth="1"/>
-    <col min="772" max="772" width="86.28515625" customWidth="1"/>
-    <col min="1028" max="1028" width="86.28515625" customWidth="1"/>
-    <col min="1284" max="1284" width="86.28515625" customWidth="1"/>
-    <col min="1540" max="1540" width="86.28515625" customWidth="1"/>
-    <col min="1796" max="1796" width="86.28515625" customWidth="1"/>
-    <col min="2052" max="2052" width="86.28515625" customWidth="1"/>
-    <col min="2308" max="2308" width="86.28515625" customWidth="1"/>
-    <col min="2564" max="2564" width="86.28515625" customWidth="1"/>
-    <col min="2820" max="2820" width="86.28515625" customWidth="1"/>
-    <col min="3076" max="3076" width="86.28515625" customWidth="1"/>
-    <col min="3332" max="3332" width="86.28515625" customWidth="1"/>
-    <col min="3588" max="3588" width="86.28515625" customWidth="1"/>
-    <col min="3844" max="3844" width="86.28515625" customWidth="1"/>
-    <col min="4100" max="4100" width="86.28515625" customWidth="1"/>
-    <col min="4356" max="4356" width="86.28515625" customWidth="1"/>
-    <col min="4612" max="4612" width="86.28515625" customWidth="1"/>
-    <col min="4868" max="4868" width="86.28515625" customWidth="1"/>
-    <col min="5124" max="5124" width="86.28515625" customWidth="1"/>
-    <col min="5380" max="5380" width="86.28515625" customWidth="1"/>
-    <col min="5636" max="5636" width="86.28515625" customWidth="1"/>
-    <col min="5892" max="5892" width="86.28515625" customWidth="1"/>
-    <col min="6148" max="6148" width="86.28515625" customWidth="1"/>
-    <col min="6404" max="6404" width="86.28515625" customWidth="1"/>
-    <col min="6660" max="6660" width="86.28515625" customWidth="1"/>
-    <col min="6916" max="6916" width="86.28515625" customWidth="1"/>
-    <col min="7172" max="7172" width="86.28515625" customWidth="1"/>
-    <col min="7428" max="7428" width="86.28515625" customWidth="1"/>
-    <col min="7684" max="7684" width="86.28515625" customWidth="1"/>
-    <col min="7940" max="7940" width="86.28515625" customWidth="1"/>
-    <col min="8196" max="8196" width="86.28515625" customWidth="1"/>
-    <col min="8452" max="8452" width="86.28515625" customWidth="1"/>
-    <col min="8708" max="8708" width="86.28515625" customWidth="1"/>
-    <col min="8964" max="8964" width="86.28515625" customWidth="1"/>
-    <col min="9220" max="9220" width="86.28515625" customWidth="1"/>
-    <col min="9476" max="9476" width="86.28515625" customWidth="1"/>
-    <col min="9732" max="9732" width="86.28515625" customWidth="1"/>
-    <col min="9988" max="9988" width="86.28515625" customWidth="1"/>
-    <col min="10244" max="10244" width="86.28515625" customWidth="1"/>
-    <col min="10500" max="10500" width="86.28515625" customWidth="1"/>
-    <col min="10756" max="10756" width="86.28515625" customWidth="1"/>
-    <col min="11012" max="11012" width="86.28515625" customWidth="1"/>
-    <col min="11268" max="11268" width="86.28515625" customWidth="1"/>
-    <col min="11524" max="11524" width="86.28515625" customWidth="1"/>
-    <col min="11780" max="11780" width="86.28515625" customWidth="1"/>
-    <col min="12036" max="12036" width="86.28515625" customWidth="1"/>
-    <col min="12292" max="12292" width="86.28515625" customWidth="1"/>
-    <col min="12548" max="12548" width="86.28515625" customWidth="1"/>
-    <col min="12804" max="12804" width="86.28515625" customWidth="1"/>
-    <col min="13060" max="13060" width="86.28515625" customWidth="1"/>
-    <col min="13316" max="13316" width="86.28515625" customWidth="1"/>
-    <col min="13572" max="13572" width="86.28515625" customWidth="1"/>
-    <col min="13828" max="13828" width="86.28515625" customWidth="1"/>
-    <col min="14084" max="14084" width="86.28515625" customWidth="1"/>
-    <col min="14340" max="14340" width="86.28515625" customWidth="1"/>
-    <col min="14596" max="14596" width="86.28515625" customWidth="1"/>
-    <col min="14852" max="14852" width="86.28515625" customWidth="1"/>
-    <col min="15108" max="15108" width="86.28515625" customWidth="1"/>
-    <col min="15364" max="15364" width="86.28515625" customWidth="1"/>
-    <col min="15620" max="15620" width="86.28515625" customWidth="1"/>
-    <col min="15876" max="15876" width="86.28515625" customWidth="1"/>
-    <col min="16132" max="16132" width="86.28515625" customWidth="1"/>
+    <col min="1" max="1" width="5.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="101.5" customWidth="1"/>
+    <col min="3" max="10" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.6640625" customWidth="1"/>
+    <col min="12" max="12" width="22.1640625" style="1" customWidth="1"/>
+    <col min="260" max="260" width="86.33203125" customWidth="1"/>
+    <col min="516" max="516" width="86.33203125" customWidth="1"/>
+    <col min="772" max="772" width="86.33203125" customWidth="1"/>
+    <col min="1028" max="1028" width="86.33203125" customWidth="1"/>
+    <col min="1284" max="1284" width="86.33203125" customWidth="1"/>
+    <col min="1540" max="1540" width="86.33203125" customWidth="1"/>
+    <col min="1796" max="1796" width="86.33203125" customWidth="1"/>
+    <col min="2052" max="2052" width="86.33203125" customWidth="1"/>
+    <col min="2308" max="2308" width="86.33203125" customWidth="1"/>
+    <col min="2564" max="2564" width="86.33203125" customWidth="1"/>
+    <col min="2820" max="2820" width="86.33203125" customWidth="1"/>
+    <col min="3076" max="3076" width="86.33203125" customWidth="1"/>
+    <col min="3332" max="3332" width="86.33203125" customWidth="1"/>
+    <col min="3588" max="3588" width="86.33203125" customWidth="1"/>
+    <col min="3844" max="3844" width="86.33203125" customWidth="1"/>
+    <col min="4100" max="4100" width="86.33203125" customWidth="1"/>
+    <col min="4356" max="4356" width="86.33203125" customWidth="1"/>
+    <col min="4612" max="4612" width="86.33203125" customWidth="1"/>
+    <col min="4868" max="4868" width="86.33203125" customWidth="1"/>
+    <col min="5124" max="5124" width="86.33203125" customWidth="1"/>
+    <col min="5380" max="5380" width="86.33203125" customWidth="1"/>
+    <col min="5636" max="5636" width="86.33203125" customWidth="1"/>
+    <col min="5892" max="5892" width="86.33203125" customWidth="1"/>
+    <col min="6148" max="6148" width="86.33203125" customWidth="1"/>
+    <col min="6404" max="6404" width="86.33203125" customWidth="1"/>
+    <col min="6660" max="6660" width="86.33203125" customWidth="1"/>
+    <col min="6916" max="6916" width="86.33203125" customWidth="1"/>
+    <col min="7172" max="7172" width="86.33203125" customWidth="1"/>
+    <col min="7428" max="7428" width="86.33203125" customWidth="1"/>
+    <col min="7684" max="7684" width="86.33203125" customWidth="1"/>
+    <col min="7940" max="7940" width="86.33203125" customWidth="1"/>
+    <col min="8196" max="8196" width="86.33203125" customWidth="1"/>
+    <col min="8452" max="8452" width="86.33203125" customWidth="1"/>
+    <col min="8708" max="8708" width="86.33203125" customWidth="1"/>
+    <col min="8964" max="8964" width="86.33203125" customWidth="1"/>
+    <col min="9220" max="9220" width="86.33203125" customWidth="1"/>
+    <col min="9476" max="9476" width="86.33203125" customWidth="1"/>
+    <col min="9732" max="9732" width="86.33203125" customWidth="1"/>
+    <col min="9988" max="9988" width="86.33203125" customWidth="1"/>
+    <col min="10244" max="10244" width="86.33203125" customWidth="1"/>
+    <col min="10500" max="10500" width="86.33203125" customWidth="1"/>
+    <col min="10756" max="10756" width="86.33203125" customWidth="1"/>
+    <col min="11012" max="11012" width="86.33203125" customWidth="1"/>
+    <col min="11268" max="11268" width="86.33203125" customWidth="1"/>
+    <col min="11524" max="11524" width="86.33203125" customWidth="1"/>
+    <col min="11780" max="11780" width="86.33203125" customWidth="1"/>
+    <col min="12036" max="12036" width="86.33203125" customWidth="1"/>
+    <col min="12292" max="12292" width="86.33203125" customWidth="1"/>
+    <col min="12548" max="12548" width="86.33203125" customWidth="1"/>
+    <col min="12804" max="12804" width="86.33203125" customWidth="1"/>
+    <col min="13060" max="13060" width="86.33203125" customWidth="1"/>
+    <col min="13316" max="13316" width="86.33203125" customWidth="1"/>
+    <col min="13572" max="13572" width="86.33203125" customWidth="1"/>
+    <col min="13828" max="13828" width="86.33203125" customWidth="1"/>
+    <col min="14084" max="14084" width="86.33203125" customWidth="1"/>
+    <col min="14340" max="14340" width="86.33203125" customWidth="1"/>
+    <col min="14596" max="14596" width="86.33203125" customWidth="1"/>
+    <col min="14852" max="14852" width="86.33203125" customWidth="1"/>
+    <col min="15108" max="15108" width="86.33203125" customWidth="1"/>
+    <col min="15364" max="15364" width="86.33203125" customWidth="1"/>
+    <col min="15620" max="15620" width="86.33203125" customWidth="1"/>
+    <col min="15876" max="15876" width="86.33203125" customWidth="1"/>
+    <col min="16132" max="16132" width="86.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:12" ht="71.25" customHeight="1">
+      <c r="A1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="16"/>
       <c r="C1" s="6" t="s">
         <v>1</v>
       </c>
@@ -929,27 +935,27 @@
       <c r="K1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="9" t="s">
+      <c r="L1" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="7" t="s">
+    <row r="2" spans="1:12" ht="18.75" customHeight="1">
+      <c r="A2" s="16"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="9"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="17"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -969,7 +975,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -989,7 +995,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -1009,7 +1015,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -1029,7 +1035,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" s="2">
         <v>5</v>
       </c>
@@ -1049,7 +1055,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" s="2">
         <v>6</v>
       </c>
@@ -1069,7 +1075,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" s="2">
         <v>7</v>
       </c>
@@ -1089,7 +1095,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="2">
         <v>8</v>
       </c>
@@ -1109,7 +1115,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" s="2">
         <v>9</v>
       </c>
@@ -1129,7 +1135,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12">
       <c r="A12" s="2">
         <v>10</v>
       </c>
@@ -1149,7 +1155,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12">
       <c r="A13" s="2">
         <v>11</v>
       </c>
@@ -1169,7 +1175,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12">
       <c r="A14" s="2">
         <v>12</v>
       </c>
@@ -1189,7 +1195,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12">
       <c r="A15" s="2">
         <v>13</v>
       </c>
@@ -1209,7 +1215,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12">
       <c r="A16" s="2">
         <v>14</v>
       </c>
@@ -1229,7 +1235,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12">
       <c r="A17" s="2">
         <v>15</v>
       </c>
@@ -1249,7 +1255,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -1269,7 +1275,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -1289,7 +1295,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -1309,7 +1315,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -1329,7 +1335,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -1349,7 +1355,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -1369,7 +1375,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -1407,524 +1413,537 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.140625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" style="11" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" style="12" customWidth="1"/>
-    <col min="4" max="4" width="30.42578125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="34" style="11" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" style="11" customWidth="1"/>
-    <col min="7" max="256" width="8.85546875" style="11"/>
-    <col min="257" max="257" width="15.140625" style="11" customWidth="1"/>
-    <col min="258" max="258" width="22.42578125" style="11" customWidth="1"/>
-    <col min="259" max="259" width="26.7109375" style="11" customWidth="1"/>
-    <col min="260" max="260" width="30.42578125" style="11" customWidth="1"/>
-    <col min="261" max="261" width="34" style="11" customWidth="1"/>
-    <col min="262" max="262" width="24.7109375" style="11" customWidth="1"/>
-    <col min="263" max="512" width="8.85546875" style="11"/>
-    <col min="513" max="513" width="15.140625" style="11" customWidth="1"/>
-    <col min="514" max="514" width="22.42578125" style="11" customWidth="1"/>
-    <col min="515" max="515" width="26.7109375" style="11" customWidth="1"/>
-    <col min="516" max="516" width="30.42578125" style="11" customWidth="1"/>
-    <col min="517" max="517" width="34" style="11" customWidth="1"/>
-    <col min="518" max="518" width="24.7109375" style="11" customWidth="1"/>
-    <col min="519" max="768" width="8.85546875" style="11"/>
-    <col min="769" max="769" width="15.140625" style="11" customWidth="1"/>
-    <col min="770" max="770" width="22.42578125" style="11" customWidth="1"/>
-    <col min="771" max="771" width="26.7109375" style="11" customWidth="1"/>
-    <col min="772" max="772" width="30.42578125" style="11" customWidth="1"/>
-    <col min="773" max="773" width="34" style="11" customWidth="1"/>
-    <col min="774" max="774" width="24.7109375" style="11" customWidth="1"/>
-    <col min="775" max="1024" width="8.85546875" style="11"/>
-    <col min="1025" max="1025" width="15.140625" style="11" customWidth="1"/>
-    <col min="1026" max="1026" width="22.42578125" style="11" customWidth="1"/>
-    <col min="1027" max="1027" width="26.7109375" style="11" customWidth="1"/>
-    <col min="1028" max="1028" width="30.42578125" style="11" customWidth="1"/>
-    <col min="1029" max="1029" width="34" style="11" customWidth="1"/>
-    <col min="1030" max="1030" width="24.7109375" style="11" customWidth="1"/>
-    <col min="1031" max="1280" width="8.85546875" style="11"/>
-    <col min="1281" max="1281" width="15.140625" style="11" customWidth="1"/>
-    <col min="1282" max="1282" width="22.42578125" style="11" customWidth="1"/>
-    <col min="1283" max="1283" width="26.7109375" style="11" customWidth="1"/>
-    <col min="1284" max="1284" width="30.42578125" style="11" customWidth="1"/>
-    <col min="1285" max="1285" width="34" style="11" customWidth="1"/>
-    <col min="1286" max="1286" width="24.7109375" style="11" customWidth="1"/>
-    <col min="1287" max="1536" width="8.85546875" style="11"/>
-    <col min="1537" max="1537" width="15.140625" style="11" customWidth="1"/>
-    <col min="1538" max="1538" width="22.42578125" style="11" customWidth="1"/>
-    <col min="1539" max="1539" width="26.7109375" style="11" customWidth="1"/>
-    <col min="1540" max="1540" width="30.42578125" style="11" customWidth="1"/>
-    <col min="1541" max="1541" width="34" style="11" customWidth="1"/>
-    <col min="1542" max="1542" width="24.7109375" style="11" customWidth="1"/>
-    <col min="1543" max="1792" width="8.85546875" style="11"/>
-    <col min="1793" max="1793" width="15.140625" style="11" customWidth="1"/>
-    <col min="1794" max="1794" width="22.42578125" style="11" customWidth="1"/>
-    <col min="1795" max="1795" width="26.7109375" style="11" customWidth="1"/>
-    <col min="1796" max="1796" width="30.42578125" style="11" customWidth="1"/>
-    <col min="1797" max="1797" width="34" style="11" customWidth="1"/>
-    <col min="1798" max="1798" width="24.7109375" style="11" customWidth="1"/>
-    <col min="1799" max="2048" width="8.85546875" style="11"/>
-    <col min="2049" max="2049" width="15.140625" style="11" customWidth="1"/>
-    <col min="2050" max="2050" width="22.42578125" style="11" customWidth="1"/>
-    <col min="2051" max="2051" width="26.7109375" style="11" customWidth="1"/>
-    <col min="2052" max="2052" width="30.42578125" style="11" customWidth="1"/>
-    <col min="2053" max="2053" width="34" style="11" customWidth="1"/>
-    <col min="2054" max="2054" width="24.7109375" style="11" customWidth="1"/>
-    <col min="2055" max="2304" width="8.85546875" style="11"/>
-    <col min="2305" max="2305" width="15.140625" style="11" customWidth="1"/>
-    <col min="2306" max="2306" width="22.42578125" style="11" customWidth="1"/>
-    <col min="2307" max="2307" width="26.7109375" style="11" customWidth="1"/>
-    <col min="2308" max="2308" width="30.42578125" style="11" customWidth="1"/>
-    <col min="2309" max="2309" width="34" style="11" customWidth="1"/>
-    <col min="2310" max="2310" width="24.7109375" style="11" customWidth="1"/>
-    <col min="2311" max="2560" width="8.85546875" style="11"/>
-    <col min="2561" max="2561" width="15.140625" style="11" customWidth="1"/>
-    <col min="2562" max="2562" width="22.42578125" style="11" customWidth="1"/>
-    <col min="2563" max="2563" width="26.7109375" style="11" customWidth="1"/>
-    <col min="2564" max="2564" width="30.42578125" style="11" customWidth="1"/>
-    <col min="2565" max="2565" width="34" style="11" customWidth="1"/>
-    <col min="2566" max="2566" width="24.7109375" style="11" customWidth="1"/>
-    <col min="2567" max="2816" width="8.85546875" style="11"/>
-    <col min="2817" max="2817" width="15.140625" style="11" customWidth="1"/>
-    <col min="2818" max="2818" width="22.42578125" style="11" customWidth="1"/>
-    <col min="2819" max="2819" width="26.7109375" style="11" customWidth="1"/>
-    <col min="2820" max="2820" width="30.42578125" style="11" customWidth="1"/>
-    <col min="2821" max="2821" width="34" style="11" customWidth="1"/>
-    <col min="2822" max="2822" width="24.7109375" style="11" customWidth="1"/>
-    <col min="2823" max="3072" width="8.85546875" style="11"/>
-    <col min="3073" max="3073" width="15.140625" style="11" customWidth="1"/>
-    <col min="3074" max="3074" width="22.42578125" style="11" customWidth="1"/>
-    <col min="3075" max="3075" width="26.7109375" style="11" customWidth="1"/>
-    <col min="3076" max="3076" width="30.42578125" style="11" customWidth="1"/>
-    <col min="3077" max="3077" width="34" style="11" customWidth="1"/>
-    <col min="3078" max="3078" width="24.7109375" style="11" customWidth="1"/>
-    <col min="3079" max="3328" width="8.85546875" style="11"/>
-    <col min="3329" max="3329" width="15.140625" style="11" customWidth="1"/>
-    <col min="3330" max="3330" width="22.42578125" style="11" customWidth="1"/>
-    <col min="3331" max="3331" width="26.7109375" style="11" customWidth="1"/>
-    <col min="3332" max="3332" width="30.42578125" style="11" customWidth="1"/>
-    <col min="3333" max="3333" width="34" style="11" customWidth="1"/>
-    <col min="3334" max="3334" width="24.7109375" style="11" customWidth="1"/>
-    <col min="3335" max="3584" width="8.85546875" style="11"/>
-    <col min="3585" max="3585" width="15.140625" style="11" customWidth="1"/>
-    <col min="3586" max="3586" width="22.42578125" style="11" customWidth="1"/>
-    <col min="3587" max="3587" width="26.7109375" style="11" customWidth="1"/>
-    <col min="3588" max="3588" width="30.42578125" style="11" customWidth="1"/>
-    <col min="3589" max="3589" width="34" style="11" customWidth="1"/>
-    <col min="3590" max="3590" width="24.7109375" style="11" customWidth="1"/>
-    <col min="3591" max="3840" width="8.85546875" style="11"/>
-    <col min="3841" max="3841" width="15.140625" style="11" customWidth="1"/>
-    <col min="3842" max="3842" width="22.42578125" style="11" customWidth="1"/>
-    <col min="3843" max="3843" width="26.7109375" style="11" customWidth="1"/>
-    <col min="3844" max="3844" width="30.42578125" style="11" customWidth="1"/>
-    <col min="3845" max="3845" width="34" style="11" customWidth="1"/>
-    <col min="3846" max="3846" width="24.7109375" style="11" customWidth="1"/>
-    <col min="3847" max="4096" width="8.85546875" style="11"/>
-    <col min="4097" max="4097" width="15.140625" style="11" customWidth="1"/>
-    <col min="4098" max="4098" width="22.42578125" style="11" customWidth="1"/>
-    <col min="4099" max="4099" width="26.7109375" style="11" customWidth="1"/>
-    <col min="4100" max="4100" width="30.42578125" style="11" customWidth="1"/>
-    <col min="4101" max="4101" width="34" style="11" customWidth="1"/>
-    <col min="4102" max="4102" width="24.7109375" style="11" customWidth="1"/>
-    <col min="4103" max="4352" width="8.85546875" style="11"/>
-    <col min="4353" max="4353" width="15.140625" style="11" customWidth="1"/>
-    <col min="4354" max="4354" width="22.42578125" style="11" customWidth="1"/>
-    <col min="4355" max="4355" width="26.7109375" style="11" customWidth="1"/>
-    <col min="4356" max="4356" width="30.42578125" style="11" customWidth="1"/>
-    <col min="4357" max="4357" width="34" style="11" customWidth="1"/>
-    <col min="4358" max="4358" width="24.7109375" style="11" customWidth="1"/>
-    <col min="4359" max="4608" width="8.85546875" style="11"/>
-    <col min="4609" max="4609" width="15.140625" style="11" customWidth="1"/>
-    <col min="4610" max="4610" width="22.42578125" style="11" customWidth="1"/>
-    <col min="4611" max="4611" width="26.7109375" style="11" customWidth="1"/>
-    <col min="4612" max="4612" width="30.42578125" style="11" customWidth="1"/>
-    <col min="4613" max="4613" width="34" style="11" customWidth="1"/>
-    <col min="4614" max="4614" width="24.7109375" style="11" customWidth="1"/>
-    <col min="4615" max="4864" width="8.85546875" style="11"/>
-    <col min="4865" max="4865" width="15.140625" style="11" customWidth="1"/>
-    <col min="4866" max="4866" width="22.42578125" style="11" customWidth="1"/>
-    <col min="4867" max="4867" width="26.7109375" style="11" customWidth="1"/>
-    <col min="4868" max="4868" width="30.42578125" style="11" customWidth="1"/>
-    <col min="4869" max="4869" width="34" style="11" customWidth="1"/>
-    <col min="4870" max="4870" width="24.7109375" style="11" customWidth="1"/>
-    <col min="4871" max="5120" width="8.85546875" style="11"/>
-    <col min="5121" max="5121" width="15.140625" style="11" customWidth="1"/>
-    <col min="5122" max="5122" width="22.42578125" style="11" customWidth="1"/>
-    <col min="5123" max="5123" width="26.7109375" style="11" customWidth="1"/>
-    <col min="5124" max="5124" width="30.42578125" style="11" customWidth="1"/>
-    <col min="5125" max="5125" width="34" style="11" customWidth="1"/>
-    <col min="5126" max="5126" width="24.7109375" style="11" customWidth="1"/>
-    <col min="5127" max="5376" width="8.85546875" style="11"/>
-    <col min="5377" max="5377" width="15.140625" style="11" customWidth="1"/>
-    <col min="5378" max="5378" width="22.42578125" style="11" customWidth="1"/>
-    <col min="5379" max="5379" width="26.7109375" style="11" customWidth="1"/>
-    <col min="5380" max="5380" width="30.42578125" style="11" customWidth="1"/>
-    <col min="5381" max="5381" width="34" style="11" customWidth="1"/>
-    <col min="5382" max="5382" width="24.7109375" style="11" customWidth="1"/>
-    <col min="5383" max="5632" width="8.85546875" style="11"/>
-    <col min="5633" max="5633" width="15.140625" style="11" customWidth="1"/>
-    <col min="5634" max="5634" width="22.42578125" style="11" customWidth="1"/>
-    <col min="5635" max="5635" width="26.7109375" style="11" customWidth="1"/>
-    <col min="5636" max="5636" width="30.42578125" style="11" customWidth="1"/>
-    <col min="5637" max="5637" width="34" style="11" customWidth="1"/>
-    <col min="5638" max="5638" width="24.7109375" style="11" customWidth="1"/>
-    <col min="5639" max="5888" width="8.85546875" style="11"/>
-    <col min="5889" max="5889" width="15.140625" style="11" customWidth="1"/>
-    <col min="5890" max="5890" width="22.42578125" style="11" customWidth="1"/>
-    <col min="5891" max="5891" width="26.7109375" style="11" customWidth="1"/>
-    <col min="5892" max="5892" width="30.42578125" style="11" customWidth="1"/>
-    <col min="5893" max="5893" width="34" style="11" customWidth="1"/>
-    <col min="5894" max="5894" width="24.7109375" style="11" customWidth="1"/>
-    <col min="5895" max="6144" width="8.85546875" style="11"/>
-    <col min="6145" max="6145" width="15.140625" style="11" customWidth="1"/>
-    <col min="6146" max="6146" width="22.42578125" style="11" customWidth="1"/>
-    <col min="6147" max="6147" width="26.7109375" style="11" customWidth="1"/>
-    <col min="6148" max="6148" width="30.42578125" style="11" customWidth="1"/>
-    <col min="6149" max="6149" width="34" style="11" customWidth="1"/>
-    <col min="6150" max="6150" width="24.7109375" style="11" customWidth="1"/>
-    <col min="6151" max="6400" width="8.85546875" style="11"/>
-    <col min="6401" max="6401" width="15.140625" style="11" customWidth="1"/>
-    <col min="6402" max="6402" width="22.42578125" style="11" customWidth="1"/>
-    <col min="6403" max="6403" width="26.7109375" style="11" customWidth="1"/>
-    <col min="6404" max="6404" width="30.42578125" style="11" customWidth="1"/>
-    <col min="6405" max="6405" width="34" style="11" customWidth="1"/>
-    <col min="6406" max="6406" width="24.7109375" style="11" customWidth="1"/>
-    <col min="6407" max="6656" width="8.85546875" style="11"/>
-    <col min="6657" max="6657" width="15.140625" style="11" customWidth="1"/>
-    <col min="6658" max="6658" width="22.42578125" style="11" customWidth="1"/>
-    <col min="6659" max="6659" width="26.7109375" style="11" customWidth="1"/>
-    <col min="6660" max="6660" width="30.42578125" style="11" customWidth="1"/>
-    <col min="6661" max="6661" width="34" style="11" customWidth="1"/>
-    <col min="6662" max="6662" width="24.7109375" style="11" customWidth="1"/>
-    <col min="6663" max="6912" width="8.85546875" style="11"/>
-    <col min="6913" max="6913" width="15.140625" style="11" customWidth="1"/>
-    <col min="6914" max="6914" width="22.42578125" style="11" customWidth="1"/>
-    <col min="6915" max="6915" width="26.7109375" style="11" customWidth="1"/>
-    <col min="6916" max="6916" width="30.42578125" style="11" customWidth="1"/>
-    <col min="6917" max="6917" width="34" style="11" customWidth="1"/>
-    <col min="6918" max="6918" width="24.7109375" style="11" customWidth="1"/>
-    <col min="6919" max="7168" width="8.85546875" style="11"/>
-    <col min="7169" max="7169" width="15.140625" style="11" customWidth="1"/>
-    <col min="7170" max="7170" width="22.42578125" style="11" customWidth="1"/>
-    <col min="7171" max="7171" width="26.7109375" style="11" customWidth="1"/>
-    <col min="7172" max="7172" width="30.42578125" style="11" customWidth="1"/>
-    <col min="7173" max="7173" width="34" style="11" customWidth="1"/>
-    <col min="7174" max="7174" width="24.7109375" style="11" customWidth="1"/>
-    <col min="7175" max="7424" width="8.85546875" style="11"/>
-    <col min="7425" max="7425" width="15.140625" style="11" customWidth="1"/>
-    <col min="7426" max="7426" width="22.42578125" style="11" customWidth="1"/>
-    <col min="7427" max="7427" width="26.7109375" style="11" customWidth="1"/>
-    <col min="7428" max="7428" width="30.42578125" style="11" customWidth="1"/>
-    <col min="7429" max="7429" width="34" style="11" customWidth="1"/>
-    <col min="7430" max="7430" width="24.7109375" style="11" customWidth="1"/>
-    <col min="7431" max="7680" width="8.85546875" style="11"/>
-    <col min="7681" max="7681" width="15.140625" style="11" customWidth="1"/>
-    <col min="7682" max="7682" width="22.42578125" style="11" customWidth="1"/>
-    <col min="7683" max="7683" width="26.7109375" style="11" customWidth="1"/>
-    <col min="7684" max="7684" width="30.42578125" style="11" customWidth="1"/>
-    <col min="7685" max="7685" width="34" style="11" customWidth="1"/>
-    <col min="7686" max="7686" width="24.7109375" style="11" customWidth="1"/>
-    <col min="7687" max="7936" width="8.85546875" style="11"/>
-    <col min="7937" max="7937" width="15.140625" style="11" customWidth="1"/>
-    <col min="7938" max="7938" width="22.42578125" style="11" customWidth="1"/>
-    <col min="7939" max="7939" width="26.7109375" style="11" customWidth="1"/>
-    <col min="7940" max="7940" width="30.42578125" style="11" customWidth="1"/>
-    <col min="7941" max="7941" width="34" style="11" customWidth="1"/>
-    <col min="7942" max="7942" width="24.7109375" style="11" customWidth="1"/>
-    <col min="7943" max="8192" width="8.85546875" style="11"/>
-    <col min="8193" max="8193" width="15.140625" style="11" customWidth="1"/>
-    <col min="8194" max="8194" width="22.42578125" style="11" customWidth="1"/>
-    <col min="8195" max="8195" width="26.7109375" style="11" customWidth="1"/>
-    <col min="8196" max="8196" width="30.42578125" style="11" customWidth="1"/>
-    <col min="8197" max="8197" width="34" style="11" customWidth="1"/>
-    <col min="8198" max="8198" width="24.7109375" style="11" customWidth="1"/>
-    <col min="8199" max="8448" width="8.85546875" style="11"/>
-    <col min="8449" max="8449" width="15.140625" style="11" customWidth="1"/>
-    <col min="8450" max="8450" width="22.42578125" style="11" customWidth="1"/>
-    <col min="8451" max="8451" width="26.7109375" style="11" customWidth="1"/>
-    <col min="8452" max="8452" width="30.42578125" style="11" customWidth="1"/>
-    <col min="8453" max="8453" width="34" style="11" customWidth="1"/>
-    <col min="8454" max="8454" width="24.7109375" style="11" customWidth="1"/>
-    <col min="8455" max="8704" width="8.85546875" style="11"/>
-    <col min="8705" max="8705" width="15.140625" style="11" customWidth="1"/>
-    <col min="8706" max="8706" width="22.42578125" style="11" customWidth="1"/>
-    <col min="8707" max="8707" width="26.7109375" style="11" customWidth="1"/>
-    <col min="8708" max="8708" width="30.42578125" style="11" customWidth="1"/>
-    <col min="8709" max="8709" width="34" style="11" customWidth="1"/>
-    <col min="8710" max="8710" width="24.7109375" style="11" customWidth="1"/>
-    <col min="8711" max="8960" width="8.85546875" style="11"/>
-    <col min="8961" max="8961" width="15.140625" style="11" customWidth="1"/>
-    <col min="8962" max="8962" width="22.42578125" style="11" customWidth="1"/>
-    <col min="8963" max="8963" width="26.7109375" style="11" customWidth="1"/>
-    <col min="8964" max="8964" width="30.42578125" style="11" customWidth="1"/>
-    <col min="8965" max="8965" width="34" style="11" customWidth="1"/>
-    <col min="8966" max="8966" width="24.7109375" style="11" customWidth="1"/>
-    <col min="8967" max="9216" width="8.85546875" style="11"/>
-    <col min="9217" max="9217" width="15.140625" style="11" customWidth="1"/>
-    <col min="9218" max="9218" width="22.42578125" style="11" customWidth="1"/>
-    <col min="9219" max="9219" width="26.7109375" style="11" customWidth="1"/>
-    <col min="9220" max="9220" width="30.42578125" style="11" customWidth="1"/>
-    <col min="9221" max="9221" width="34" style="11" customWidth="1"/>
-    <col min="9222" max="9222" width="24.7109375" style="11" customWidth="1"/>
-    <col min="9223" max="9472" width="8.85546875" style="11"/>
-    <col min="9473" max="9473" width="15.140625" style="11" customWidth="1"/>
-    <col min="9474" max="9474" width="22.42578125" style="11" customWidth="1"/>
-    <col min="9475" max="9475" width="26.7109375" style="11" customWidth="1"/>
-    <col min="9476" max="9476" width="30.42578125" style="11" customWidth="1"/>
-    <col min="9477" max="9477" width="34" style="11" customWidth="1"/>
-    <col min="9478" max="9478" width="24.7109375" style="11" customWidth="1"/>
-    <col min="9479" max="9728" width="8.85546875" style="11"/>
-    <col min="9729" max="9729" width="15.140625" style="11" customWidth="1"/>
-    <col min="9730" max="9730" width="22.42578125" style="11" customWidth="1"/>
-    <col min="9731" max="9731" width="26.7109375" style="11" customWidth="1"/>
-    <col min="9732" max="9732" width="30.42578125" style="11" customWidth="1"/>
-    <col min="9733" max="9733" width="34" style="11" customWidth="1"/>
-    <col min="9734" max="9734" width="24.7109375" style="11" customWidth="1"/>
-    <col min="9735" max="9984" width="8.85546875" style="11"/>
-    <col min="9985" max="9985" width="15.140625" style="11" customWidth="1"/>
-    <col min="9986" max="9986" width="22.42578125" style="11" customWidth="1"/>
-    <col min="9987" max="9987" width="26.7109375" style="11" customWidth="1"/>
-    <col min="9988" max="9988" width="30.42578125" style="11" customWidth="1"/>
-    <col min="9989" max="9989" width="34" style="11" customWidth="1"/>
-    <col min="9990" max="9990" width="24.7109375" style="11" customWidth="1"/>
-    <col min="9991" max="10240" width="8.85546875" style="11"/>
-    <col min="10241" max="10241" width="15.140625" style="11" customWidth="1"/>
-    <col min="10242" max="10242" width="22.42578125" style="11" customWidth="1"/>
-    <col min="10243" max="10243" width="26.7109375" style="11" customWidth="1"/>
-    <col min="10244" max="10244" width="30.42578125" style="11" customWidth="1"/>
-    <col min="10245" max="10245" width="34" style="11" customWidth="1"/>
-    <col min="10246" max="10246" width="24.7109375" style="11" customWidth="1"/>
-    <col min="10247" max="10496" width="8.85546875" style="11"/>
-    <col min="10497" max="10497" width="15.140625" style="11" customWidth="1"/>
-    <col min="10498" max="10498" width="22.42578125" style="11" customWidth="1"/>
-    <col min="10499" max="10499" width="26.7109375" style="11" customWidth="1"/>
-    <col min="10500" max="10500" width="30.42578125" style="11" customWidth="1"/>
-    <col min="10501" max="10501" width="34" style="11" customWidth="1"/>
-    <col min="10502" max="10502" width="24.7109375" style="11" customWidth="1"/>
-    <col min="10503" max="10752" width="8.85546875" style="11"/>
-    <col min="10753" max="10753" width="15.140625" style="11" customWidth="1"/>
-    <col min="10754" max="10754" width="22.42578125" style="11" customWidth="1"/>
-    <col min="10755" max="10755" width="26.7109375" style="11" customWidth="1"/>
-    <col min="10756" max="10756" width="30.42578125" style="11" customWidth="1"/>
-    <col min="10757" max="10757" width="34" style="11" customWidth="1"/>
-    <col min="10758" max="10758" width="24.7109375" style="11" customWidth="1"/>
-    <col min="10759" max="11008" width="8.85546875" style="11"/>
-    <col min="11009" max="11009" width="15.140625" style="11" customWidth="1"/>
-    <col min="11010" max="11010" width="22.42578125" style="11" customWidth="1"/>
-    <col min="11011" max="11011" width="26.7109375" style="11" customWidth="1"/>
-    <col min="11012" max="11012" width="30.42578125" style="11" customWidth="1"/>
-    <col min="11013" max="11013" width="34" style="11" customWidth="1"/>
-    <col min="11014" max="11014" width="24.7109375" style="11" customWidth="1"/>
-    <col min="11015" max="11264" width="8.85546875" style="11"/>
-    <col min="11265" max="11265" width="15.140625" style="11" customWidth="1"/>
-    <col min="11266" max="11266" width="22.42578125" style="11" customWidth="1"/>
-    <col min="11267" max="11267" width="26.7109375" style="11" customWidth="1"/>
-    <col min="11268" max="11268" width="30.42578125" style="11" customWidth="1"/>
-    <col min="11269" max="11269" width="34" style="11" customWidth="1"/>
-    <col min="11270" max="11270" width="24.7109375" style="11" customWidth="1"/>
-    <col min="11271" max="11520" width="8.85546875" style="11"/>
-    <col min="11521" max="11521" width="15.140625" style="11" customWidth="1"/>
-    <col min="11522" max="11522" width="22.42578125" style="11" customWidth="1"/>
-    <col min="11523" max="11523" width="26.7109375" style="11" customWidth="1"/>
-    <col min="11524" max="11524" width="30.42578125" style="11" customWidth="1"/>
-    <col min="11525" max="11525" width="34" style="11" customWidth="1"/>
-    <col min="11526" max="11526" width="24.7109375" style="11" customWidth="1"/>
-    <col min="11527" max="11776" width="8.85546875" style="11"/>
-    <col min="11777" max="11777" width="15.140625" style="11" customWidth="1"/>
-    <col min="11778" max="11778" width="22.42578125" style="11" customWidth="1"/>
-    <col min="11779" max="11779" width="26.7109375" style="11" customWidth="1"/>
-    <col min="11780" max="11780" width="30.42578125" style="11" customWidth="1"/>
-    <col min="11781" max="11781" width="34" style="11" customWidth="1"/>
-    <col min="11782" max="11782" width="24.7109375" style="11" customWidth="1"/>
-    <col min="11783" max="12032" width="8.85546875" style="11"/>
-    <col min="12033" max="12033" width="15.140625" style="11" customWidth="1"/>
-    <col min="12034" max="12034" width="22.42578125" style="11" customWidth="1"/>
-    <col min="12035" max="12035" width="26.7109375" style="11" customWidth="1"/>
-    <col min="12036" max="12036" width="30.42578125" style="11" customWidth="1"/>
-    <col min="12037" max="12037" width="34" style="11" customWidth="1"/>
-    <col min="12038" max="12038" width="24.7109375" style="11" customWidth="1"/>
-    <col min="12039" max="12288" width="8.85546875" style="11"/>
-    <col min="12289" max="12289" width="15.140625" style="11" customWidth="1"/>
-    <col min="12290" max="12290" width="22.42578125" style="11" customWidth="1"/>
-    <col min="12291" max="12291" width="26.7109375" style="11" customWidth="1"/>
-    <col min="12292" max="12292" width="30.42578125" style="11" customWidth="1"/>
-    <col min="12293" max="12293" width="34" style="11" customWidth="1"/>
-    <col min="12294" max="12294" width="24.7109375" style="11" customWidth="1"/>
-    <col min="12295" max="12544" width="8.85546875" style="11"/>
-    <col min="12545" max="12545" width="15.140625" style="11" customWidth="1"/>
-    <col min="12546" max="12546" width="22.42578125" style="11" customWidth="1"/>
-    <col min="12547" max="12547" width="26.7109375" style="11" customWidth="1"/>
-    <col min="12548" max="12548" width="30.42578125" style="11" customWidth="1"/>
-    <col min="12549" max="12549" width="34" style="11" customWidth="1"/>
-    <col min="12550" max="12550" width="24.7109375" style="11" customWidth="1"/>
-    <col min="12551" max="12800" width="8.85546875" style="11"/>
-    <col min="12801" max="12801" width="15.140625" style="11" customWidth="1"/>
-    <col min="12802" max="12802" width="22.42578125" style="11" customWidth="1"/>
-    <col min="12803" max="12803" width="26.7109375" style="11" customWidth="1"/>
-    <col min="12804" max="12804" width="30.42578125" style="11" customWidth="1"/>
-    <col min="12805" max="12805" width="34" style="11" customWidth="1"/>
-    <col min="12806" max="12806" width="24.7109375" style="11" customWidth="1"/>
-    <col min="12807" max="13056" width="8.85546875" style="11"/>
-    <col min="13057" max="13057" width="15.140625" style="11" customWidth="1"/>
-    <col min="13058" max="13058" width="22.42578125" style="11" customWidth="1"/>
-    <col min="13059" max="13059" width="26.7109375" style="11" customWidth="1"/>
-    <col min="13060" max="13060" width="30.42578125" style="11" customWidth="1"/>
-    <col min="13061" max="13061" width="34" style="11" customWidth="1"/>
-    <col min="13062" max="13062" width="24.7109375" style="11" customWidth="1"/>
-    <col min="13063" max="13312" width="8.85546875" style="11"/>
-    <col min="13313" max="13313" width="15.140625" style="11" customWidth="1"/>
-    <col min="13314" max="13314" width="22.42578125" style="11" customWidth="1"/>
-    <col min="13315" max="13315" width="26.7109375" style="11" customWidth="1"/>
-    <col min="13316" max="13316" width="30.42578125" style="11" customWidth="1"/>
-    <col min="13317" max="13317" width="34" style="11" customWidth="1"/>
-    <col min="13318" max="13318" width="24.7109375" style="11" customWidth="1"/>
-    <col min="13319" max="13568" width="8.85546875" style="11"/>
-    <col min="13569" max="13569" width="15.140625" style="11" customWidth="1"/>
-    <col min="13570" max="13570" width="22.42578125" style="11" customWidth="1"/>
-    <col min="13571" max="13571" width="26.7109375" style="11" customWidth="1"/>
-    <col min="13572" max="13572" width="30.42578125" style="11" customWidth="1"/>
-    <col min="13573" max="13573" width="34" style="11" customWidth="1"/>
-    <col min="13574" max="13574" width="24.7109375" style="11" customWidth="1"/>
-    <col min="13575" max="13824" width="8.85546875" style="11"/>
-    <col min="13825" max="13825" width="15.140625" style="11" customWidth="1"/>
-    <col min="13826" max="13826" width="22.42578125" style="11" customWidth="1"/>
-    <col min="13827" max="13827" width="26.7109375" style="11" customWidth="1"/>
-    <col min="13828" max="13828" width="30.42578125" style="11" customWidth="1"/>
-    <col min="13829" max="13829" width="34" style="11" customWidth="1"/>
-    <col min="13830" max="13830" width="24.7109375" style="11" customWidth="1"/>
-    <col min="13831" max="14080" width="8.85546875" style="11"/>
-    <col min="14081" max="14081" width="15.140625" style="11" customWidth="1"/>
-    <col min="14082" max="14082" width="22.42578125" style="11" customWidth="1"/>
-    <col min="14083" max="14083" width="26.7109375" style="11" customWidth="1"/>
-    <col min="14084" max="14084" width="30.42578125" style="11" customWidth="1"/>
-    <col min="14085" max="14085" width="34" style="11" customWidth="1"/>
-    <col min="14086" max="14086" width="24.7109375" style="11" customWidth="1"/>
-    <col min="14087" max="14336" width="8.85546875" style="11"/>
-    <col min="14337" max="14337" width="15.140625" style="11" customWidth="1"/>
-    <col min="14338" max="14338" width="22.42578125" style="11" customWidth="1"/>
-    <col min="14339" max="14339" width="26.7109375" style="11" customWidth="1"/>
-    <col min="14340" max="14340" width="30.42578125" style="11" customWidth="1"/>
-    <col min="14341" max="14341" width="34" style="11" customWidth="1"/>
-    <col min="14342" max="14342" width="24.7109375" style="11" customWidth="1"/>
-    <col min="14343" max="14592" width="8.85546875" style="11"/>
-    <col min="14593" max="14593" width="15.140625" style="11" customWidth="1"/>
-    <col min="14594" max="14594" width="22.42578125" style="11" customWidth="1"/>
-    <col min="14595" max="14595" width="26.7109375" style="11" customWidth="1"/>
-    <col min="14596" max="14596" width="30.42578125" style="11" customWidth="1"/>
-    <col min="14597" max="14597" width="34" style="11" customWidth="1"/>
-    <col min="14598" max="14598" width="24.7109375" style="11" customWidth="1"/>
-    <col min="14599" max="14848" width="8.85546875" style="11"/>
-    <col min="14849" max="14849" width="15.140625" style="11" customWidth="1"/>
-    <col min="14850" max="14850" width="22.42578125" style="11" customWidth="1"/>
-    <col min="14851" max="14851" width="26.7109375" style="11" customWidth="1"/>
-    <col min="14852" max="14852" width="30.42578125" style="11" customWidth="1"/>
-    <col min="14853" max="14853" width="34" style="11" customWidth="1"/>
-    <col min="14854" max="14854" width="24.7109375" style="11" customWidth="1"/>
-    <col min="14855" max="15104" width="8.85546875" style="11"/>
-    <col min="15105" max="15105" width="15.140625" style="11" customWidth="1"/>
-    <col min="15106" max="15106" width="22.42578125" style="11" customWidth="1"/>
-    <col min="15107" max="15107" width="26.7109375" style="11" customWidth="1"/>
-    <col min="15108" max="15108" width="30.42578125" style="11" customWidth="1"/>
-    <col min="15109" max="15109" width="34" style="11" customWidth="1"/>
-    <col min="15110" max="15110" width="24.7109375" style="11" customWidth="1"/>
-    <col min="15111" max="15360" width="8.85546875" style="11"/>
-    <col min="15361" max="15361" width="15.140625" style="11" customWidth="1"/>
-    <col min="15362" max="15362" width="22.42578125" style="11" customWidth="1"/>
-    <col min="15363" max="15363" width="26.7109375" style="11" customWidth="1"/>
-    <col min="15364" max="15364" width="30.42578125" style="11" customWidth="1"/>
-    <col min="15365" max="15365" width="34" style="11" customWidth="1"/>
-    <col min="15366" max="15366" width="24.7109375" style="11" customWidth="1"/>
-    <col min="15367" max="15616" width="8.85546875" style="11"/>
-    <col min="15617" max="15617" width="15.140625" style="11" customWidth="1"/>
-    <col min="15618" max="15618" width="22.42578125" style="11" customWidth="1"/>
-    <col min="15619" max="15619" width="26.7109375" style="11" customWidth="1"/>
-    <col min="15620" max="15620" width="30.42578125" style="11" customWidth="1"/>
-    <col min="15621" max="15621" width="34" style="11" customWidth="1"/>
-    <col min="15622" max="15622" width="24.7109375" style="11" customWidth="1"/>
-    <col min="15623" max="15872" width="8.85546875" style="11"/>
-    <col min="15873" max="15873" width="15.140625" style="11" customWidth="1"/>
-    <col min="15874" max="15874" width="22.42578125" style="11" customWidth="1"/>
-    <col min="15875" max="15875" width="26.7109375" style="11" customWidth="1"/>
-    <col min="15876" max="15876" width="30.42578125" style="11" customWidth="1"/>
-    <col min="15877" max="15877" width="34" style="11" customWidth="1"/>
-    <col min="15878" max="15878" width="24.7109375" style="11" customWidth="1"/>
-    <col min="15879" max="16128" width="8.85546875" style="11"/>
-    <col min="16129" max="16129" width="15.140625" style="11" customWidth="1"/>
-    <col min="16130" max="16130" width="22.42578125" style="11" customWidth="1"/>
-    <col min="16131" max="16131" width="26.7109375" style="11" customWidth="1"/>
-    <col min="16132" max="16132" width="30.42578125" style="11" customWidth="1"/>
-    <col min="16133" max="16133" width="34" style="11" customWidth="1"/>
-    <col min="16134" max="16134" width="24.7109375" style="11" customWidth="1"/>
-    <col min="16135" max="16384" width="8.85546875" style="11"/>
+    <col min="1" max="1" width="15.1640625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="22.5" style="8" customWidth="1"/>
+    <col min="3" max="3" width="41.33203125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="30.5" style="9" customWidth="1"/>
+    <col min="5" max="5" width="34" style="8" customWidth="1"/>
+    <col min="6" max="6" width="24.6640625" style="8" customWidth="1"/>
+    <col min="7" max="256" width="8.83203125" style="8"/>
+    <col min="257" max="257" width="15.1640625" style="8" customWidth="1"/>
+    <col min="258" max="258" width="22.5" style="8" customWidth="1"/>
+    <col min="259" max="259" width="26.6640625" style="8" customWidth="1"/>
+    <col min="260" max="260" width="30.5" style="8" customWidth="1"/>
+    <col min="261" max="261" width="34" style="8" customWidth="1"/>
+    <col min="262" max="262" width="24.6640625" style="8" customWidth="1"/>
+    <col min="263" max="512" width="8.83203125" style="8"/>
+    <col min="513" max="513" width="15.1640625" style="8" customWidth="1"/>
+    <col min="514" max="514" width="22.5" style="8" customWidth="1"/>
+    <col min="515" max="515" width="26.6640625" style="8" customWidth="1"/>
+    <col min="516" max="516" width="30.5" style="8" customWidth="1"/>
+    <col min="517" max="517" width="34" style="8" customWidth="1"/>
+    <col min="518" max="518" width="24.6640625" style="8" customWidth="1"/>
+    <col min="519" max="768" width="8.83203125" style="8"/>
+    <col min="769" max="769" width="15.1640625" style="8" customWidth="1"/>
+    <col min="770" max="770" width="22.5" style="8" customWidth="1"/>
+    <col min="771" max="771" width="26.6640625" style="8" customWidth="1"/>
+    <col min="772" max="772" width="30.5" style="8" customWidth="1"/>
+    <col min="773" max="773" width="34" style="8" customWidth="1"/>
+    <col min="774" max="774" width="24.6640625" style="8" customWidth="1"/>
+    <col min="775" max="1024" width="8.83203125" style="8"/>
+    <col min="1025" max="1025" width="15.1640625" style="8" customWidth="1"/>
+    <col min="1026" max="1026" width="22.5" style="8" customWidth="1"/>
+    <col min="1027" max="1027" width="26.6640625" style="8" customWidth="1"/>
+    <col min="1028" max="1028" width="30.5" style="8" customWidth="1"/>
+    <col min="1029" max="1029" width="34" style="8" customWidth="1"/>
+    <col min="1030" max="1030" width="24.6640625" style="8" customWidth="1"/>
+    <col min="1031" max="1280" width="8.83203125" style="8"/>
+    <col min="1281" max="1281" width="15.1640625" style="8" customWidth="1"/>
+    <col min="1282" max="1282" width="22.5" style="8" customWidth="1"/>
+    <col min="1283" max="1283" width="26.6640625" style="8" customWidth="1"/>
+    <col min="1284" max="1284" width="30.5" style="8" customWidth="1"/>
+    <col min="1285" max="1285" width="34" style="8" customWidth="1"/>
+    <col min="1286" max="1286" width="24.6640625" style="8" customWidth="1"/>
+    <col min="1287" max="1536" width="8.83203125" style="8"/>
+    <col min="1537" max="1537" width="15.1640625" style="8" customWidth="1"/>
+    <col min="1538" max="1538" width="22.5" style="8" customWidth="1"/>
+    <col min="1539" max="1539" width="26.6640625" style="8" customWidth="1"/>
+    <col min="1540" max="1540" width="30.5" style="8" customWidth="1"/>
+    <col min="1541" max="1541" width="34" style="8" customWidth="1"/>
+    <col min="1542" max="1542" width="24.6640625" style="8" customWidth="1"/>
+    <col min="1543" max="1792" width="8.83203125" style="8"/>
+    <col min="1793" max="1793" width="15.1640625" style="8" customWidth="1"/>
+    <col min="1794" max="1794" width="22.5" style="8" customWidth="1"/>
+    <col min="1795" max="1795" width="26.6640625" style="8" customWidth="1"/>
+    <col min="1796" max="1796" width="30.5" style="8" customWidth="1"/>
+    <col min="1797" max="1797" width="34" style="8" customWidth="1"/>
+    <col min="1798" max="1798" width="24.6640625" style="8" customWidth="1"/>
+    <col min="1799" max="2048" width="8.83203125" style="8"/>
+    <col min="2049" max="2049" width="15.1640625" style="8" customWidth="1"/>
+    <col min="2050" max="2050" width="22.5" style="8" customWidth="1"/>
+    <col min="2051" max="2051" width="26.6640625" style="8" customWidth="1"/>
+    <col min="2052" max="2052" width="30.5" style="8" customWidth="1"/>
+    <col min="2053" max="2053" width="34" style="8" customWidth="1"/>
+    <col min="2054" max="2054" width="24.6640625" style="8" customWidth="1"/>
+    <col min="2055" max="2304" width="8.83203125" style="8"/>
+    <col min="2305" max="2305" width="15.1640625" style="8" customWidth="1"/>
+    <col min="2306" max="2306" width="22.5" style="8" customWidth="1"/>
+    <col min="2307" max="2307" width="26.6640625" style="8" customWidth="1"/>
+    <col min="2308" max="2308" width="30.5" style="8" customWidth="1"/>
+    <col min="2309" max="2309" width="34" style="8" customWidth="1"/>
+    <col min="2310" max="2310" width="24.6640625" style="8" customWidth="1"/>
+    <col min="2311" max="2560" width="8.83203125" style="8"/>
+    <col min="2561" max="2561" width="15.1640625" style="8" customWidth="1"/>
+    <col min="2562" max="2562" width="22.5" style="8" customWidth="1"/>
+    <col min="2563" max="2563" width="26.6640625" style="8" customWidth="1"/>
+    <col min="2564" max="2564" width="30.5" style="8" customWidth="1"/>
+    <col min="2565" max="2565" width="34" style="8" customWidth="1"/>
+    <col min="2566" max="2566" width="24.6640625" style="8" customWidth="1"/>
+    <col min="2567" max="2816" width="8.83203125" style="8"/>
+    <col min="2817" max="2817" width="15.1640625" style="8" customWidth="1"/>
+    <col min="2818" max="2818" width="22.5" style="8" customWidth="1"/>
+    <col min="2819" max="2819" width="26.6640625" style="8" customWidth="1"/>
+    <col min="2820" max="2820" width="30.5" style="8" customWidth="1"/>
+    <col min="2821" max="2821" width="34" style="8" customWidth="1"/>
+    <col min="2822" max="2822" width="24.6640625" style="8" customWidth="1"/>
+    <col min="2823" max="3072" width="8.83203125" style="8"/>
+    <col min="3073" max="3073" width="15.1640625" style="8" customWidth="1"/>
+    <col min="3074" max="3074" width="22.5" style="8" customWidth="1"/>
+    <col min="3075" max="3075" width="26.6640625" style="8" customWidth="1"/>
+    <col min="3076" max="3076" width="30.5" style="8" customWidth="1"/>
+    <col min="3077" max="3077" width="34" style="8" customWidth="1"/>
+    <col min="3078" max="3078" width="24.6640625" style="8" customWidth="1"/>
+    <col min="3079" max="3328" width="8.83203125" style="8"/>
+    <col min="3329" max="3329" width="15.1640625" style="8" customWidth="1"/>
+    <col min="3330" max="3330" width="22.5" style="8" customWidth="1"/>
+    <col min="3331" max="3331" width="26.6640625" style="8" customWidth="1"/>
+    <col min="3332" max="3332" width="30.5" style="8" customWidth="1"/>
+    <col min="3333" max="3333" width="34" style="8" customWidth="1"/>
+    <col min="3334" max="3334" width="24.6640625" style="8" customWidth="1"/>
+    <col min="3335" max="3584" width="8.83203125" style="8"/>
+    <col min="3585" max="3585" width="15.1640625" style="8" customWidth="1"/>
+    <col min="3586" max="3586" width="22.5" style="8" customWidth="1"/>
+    <col min="3587" max="3587" width="26.6640625" style="8" customWidth="1"/>
+    <col min="3588" max="3588" width="30.5" style="8" customWidth="1"/>
+    <col min="3589" max="3589" width="34" style="8" customWidth="1"/>
+    <col min="3590" max="3590" width="24.6640625" style="8" customWidth="1"/>
+    <col min="3591" max="3840" width="8.83203125" style="8"/>
+    <col min="3841" max="3841" width="15.1640625" style="8" customWidth="1"/>
+    <col min="3842" max="3842" width="22.5" style="8" customWidth="1"/>
+    <col min="3843" max="3843" width="26.6640625" style="8" customWidth="1"/>
+    <col min="3844" max="3844" width="30.5" style="8" customWidth="1"/>
+    <col min="3845" max="3845" width="34" style="8" customWidth="1"/>
+    <col min="3846" max="3846" width="24.6640625" style="8" customWidth="1"/>
+    <col min="3847" max="4096" width="8.83203125" style="8"/>
+    <col min="4097" max="4097" width="15.1640625" style="8" customWidth="1"/>
+    <col min="4098" max="4098" width="22.5" style="8" customWidth="1"/>
+    <col min="4099" max="4099" width="26.6640625" style="8" customWidth="1"/>
+    <col min="4100" max="4100" width="30.5" style="8" customWidth="1"/>
+    <col min="4101" max="4101" width="34" style="8" customWidth="1"/>
+    <col min="4102" max="4102" width="24.6640625" style="8" customWidth="1"/>
+    <col min="4103" max="4352" width="8.83203125" style="8"/>
+    <col min="4353" max="4353" width="15.1640625" style="8" customWidth="1"/>
+    <col min="4354" max="4354" width="22.5" style="8" customWidth="1"/>
+    <col min="4355" max="4355" width="26.6640625" style="8" customWidth="1"/>
+    <col min="4356" max="4356" width="30.5" style="8" customWidth="1"/>
+    <col min="4357" max="4357" width="34" style="8" customWidth="1"/>
+    <col min="4358" max="4358" width="24.6640625" style="8" customWidth="1"/>
+    <col min="4359" max="4608" width="8.83203125" style="8"/>
+    <col min="4609" max="4609" width="15.1640625" style="8" customWidth="1"/>
+    <col min="4610" max="4610" width="22.5" style="8" customWidth="1"/>
+    <col min="4611" max="4611" width="26.6640625" style="8" customWidth="1"/>
+    <col min="4612" max="4612" width="30.5" style="8" customWidth="1"/>
+    <col min="4613" max="4613" width="34" style="8" customWidth="1"/>
+    <col min="4614" max="4614" width="24.6640625" style="8" customWidth="1"/>
+    <col min="4615" max="4864" width="8.83203125" style="8"/>
+    <col min="4865" max="4865" width="15.1640625" style="8" customWidth="1"/>
+    <col min="4866" max="4866" width="22.5" style="8" customWidth="1"/>
+    <col min="4867" max="4867" width="26.6640625" style="8" customWidth="1"/>
+    <col min="4868" max="4868" width="30.5" style="8" customWidth="1"/>
+    <col min="4869" max="4869" width="34" style="8" customWidth="1"/>
+    <col min="4870" max="4870" width="24.6640625" style="8" customWidth="1"/>
+    <col min="4871" max="5120" width="8.83203125" style="8"/>
+    <col min="5121" max="5121" width="15.1640625" style="8" customWidth="1"/>
+    <col min="5122" max="5122" width="22.5" style="8" customWidth="1"/>
+    <col min="5123" max="5123" width="26.6640625" style="8" customWidth="1"/>
+    <col min="5124" max="5124" width="30.5" style="8" customWidth="1"/>
+    <col min="5125" max="5125" width="34" style="8" customWidth="1"/>
+    <col min="5126" max="5126" width="24.6640625" style="8" customWidth="1"/>
+    <col min="5127" max="5376" width="8.83203125" style="8"/>
+    <col min="5377" max="5377" width="15.1640625" style="8" customWidth="1"/>
+    <col min="5378" max="5378" width="22.5" style="8" customWidth="1"/>
+    <col min="5379" max="5379" width="26.6640625" style="8" customWidth="1"/>
+    <col min="5380" max="5380" width="30.5" style="8" customWidth="1"/>
+    <col min="5381" max="5381" width="34" style="8" customWidth="1"/>
+    <col min="5382" max="5382" width="24.6640625" style="8" customWidth="1"/>
+    <col min="5383" max="5632" width="8.83203125" style="8"/>
+    <col min="5633" max="5633" width="15.1640625" style="8" customWidth="1"/>
+    <col min="5634" max="5634" width="22.5" style="8" customWidth="1"/>
+    <col min="5635" max="5635" width="26.6640625" style="8" customWidth="1"/>
+    <col min="5636" max="5636" width="30.5" style="8" customWidth="1"/>
+    <col min="5637" max="5637" width="34" style="8" customWidth="1"/>
+    <col min="5638" max="5638" width="24.6640625" style="8" customWidth="1"/>
+    <col min="5639" max="5888" width="8.83203125" style="8"/>
+    <col min="5889" max="5889" width="15.1640625" style="8" customWidth="1"/>
+    <col min="5890" max="5890" width="22.5" style="8" customWidth="1"/>
+    <col min="5891" max="5891" width="26.6640625" style="8" customWidth="1"/>
+    <col min="5892" max="5892" width="30.5" style="8" customWidth="1"/>
+    <col min="5893" max="5893" width="34" style="8" customWidth="1"/>
+    <col min="5894" max="5894" width="24.6640625" style="8" customWidth="1"/>
+    <col min="5895" max="6144" width="8.83203125" style="8"/>
+    <col min="6145" max="6145" width="15.1640625" style="8" customWidth="1"/>
+    <col min="6146" max="6146" width="22.5" style="8" customWidth="1"/>
+    <col min="6147" max="6147" width="26.6640625" style="8" customWidth="1"/>
+    <col min="6148" max="6148" width="30.5" style="8" customWidth="1"/>
+    <col min="6149" max="6149" width="34" style="8" customWidth="1"/>
+    <col min="6150" max="6150" width="24.6640625" style="8" customWidth="1"/>
+    <col min="6151" max="6400" width="8.83203125" style="8"/>
+    <col min="6401" max="6401" width="15.1640625" style="8" customWidth="1"/>
+    <col min="6402" max="6402" width="22.5" style="8" customWidth="1"/>
+    <col min="6403" max="6403" width="26.6640625" style="8" customWidth="1"/>
+    <col min="6404" max="6404" width="30.5" style="8" customWidth="1"/>
+    <col min="6405" max="6405" width="34" style="8" customWidth="1"/>
+    <col min="6406" max="6406" width="24.6640625" style="8" customWidth="1"/>
+    <col min="6407" max="6656" width="8.83203125" style="8"/>
+    <col min="6657" max="6657" width="15.1640625" style="8" customWidth="1"/>
+    <col min="6658" max="6658" width="22.5" style="8" customWidth="1"/>
+    <col min="6659" max="6659" width="26.6640625" style="8" customWidth="1"/>
+    <col min="6660" max="6660" width="30.5" style="8" customWidth="1"/>
+    <col min="6661" max="6661" width="34" style="8" customWidth="1"/>
+    <col min="6662" max="6662" width="24.6640625" style="8" customWidth="1"/>
+    <col min="6663" max="6912" width="8.83203125" style="8"/>
+    <col min="6913" max="6913" width="15.1640625" style="8" customWidth="1"/>
+    <col min="6914" max="6914" width="22.5" style="8" customWidth="1"/>
+    <col min="6915" max="6915" width="26.6640625" style="8" customWidth="1"/>
+    <col min="6916" max="6916" width="30.5" style="8" customWidth="1"/>
+    <col min="6917" max="6917" width="34" style="8" customWidth="1"/>
+    <col min="6918" max="6918" width="24.6640625" style="8" customWidth="1"/>
+    <col min="6919" max="7168" width="8.83203125" style="8"/>
+    <col min="7169" max="7169" width="15.1640625" style="8" customWidth="1"/>
+    <col min="7170" max="7170" width="22.5" style="8" customWidth="1"/>
+    <col min="7171" max="7171" width="26.6640625" style="8" customWidth="1"/>
+    <col min="7172" max="7172" width="30.5" style="8" customWidth="1"/>
+    <col min="7173" max="7173" width="34" style="8" customWidth="1"/>
+    <col min="7174" max="7174" width="24.6640625" style="8" customWidth="1"/>
+    <col min="7175" max="7424" width="8.83203125" style="8"/>
+    <col min="7425" max="7425" width="15.1640625" style="8" customWidth="1"/>
+    <col min="7426" max="7426" width="22.5" style="8" customWidth="1"/>
+    <col min="7427" max="7427" width="26.6640625" style="8" customWidth="1"/>
+    <col min="7428" max="7428" width="30.5" style="8" customWidth="1"/>
+    <col min="7429" max="7429" width="34" style="8" customWidth="1"/>
+    <col min="7430" max="7430" width="24.6640625" style="8" customWidth="1"/>
+    <col min="7431" max="7680" width="8.83203125" style="8"/>
+    <col min="7681" max="7681" width="15.1640625" style="8" customWidth="1"/>
+    <col min="7682" max="7682" width="22.5" style="8" customWidth="1"/>
+    <col min="7683" max="7683" width="26.6640625" style="8" customWidth="1"/>
+    <col min="7684" max="7684" width="30.5" style="8" customWidth="1"/>
+    <col min="7685" max="7685" width="34" style="8" customWidth="1"/>
+    <col min="7686" max="7686" width="24.6640625" style="8" customWidth="1"/>
+    <col min="7687" max="7936" width="8.83203125" style="8"/>
+    <col min="7937" max="7937" width="15.1640625" style="8" customWidth="1"/>
+    <col min="7938" max="7938" width="22.5" style="8" customWidth="1"/>
+    <col min="7939" max="7939" width="26.6640625" style="8" customWidth="1"/>
+    <col min="7940" max="7940" width="30.5" style="8" customWidth="1"/>
+    <col min="7941" max="7941" width="34" style="8" customWidth="1"/>
+    <col min="7942" max="7942" width="24.6640625" style="8" customWidth="1"/>
+    <col min="7943" max="8192" width="8.83203125" style="8"/>
+    <col min="8193" max="8193" width="15.1640625" style="8" customWidth="1"/>
+    <col min="8194" max="8194" width="22.5" style="8" customWidth="1"/>
+    <col min="8195" max="8195" width="26.6640625" style="8" customWidth="1"/>
+    <col min="8196" max="8196" width="30.5" style="8" customWidth="1"/>
+    <col min="8197" max="8197" width="34" style="8" customWidth="1"/>
+    <col min="8198" max="8198" width="24.6640625" style="8" customWidth="1"/>
+    <col min="8199" max="8448" width="8.83203125" style="8"/>
+    <col min="8449" max="8449" width="15.1640625" style="8" customWidth="1"/>
+    <col min="8450" max="8450" width="22.5" style="8" customWidth="1"/>
+    <col min="8451" max="8451" width="26.6640625" style="8" customWidth="1"/>
+    <col min="8452" max="8452" width="30.5" style="8" customWidth="1"/>
+    <col min="8453" max="8453" width="34" style="8" customWidth="1"/>
+    <col min="8454" max="8454" width="24.6640625" style="8" customWidth="1"/>
+    <col min="8455" max="8704" width="8.83203125" style="8"/>
+    <col min="8705" max="8705" width="15.1640625" style="8" customWidth="1"/>
+    <col min="8706" max="8706" width="22.5" style="8" customWidth="1"/>
+    <col min="8707" max="8707" width="26.6640625" style="8" customWidth="1"/>
+    <col min="8708" max="8708" width="30.5" style="8" customWidth="1"/>
+    <col min="8709" max="8709" width="34" style="8" customWidth="1"/>
+    <col min="8710" max="8710" width="24.6640625" style="8" customWidth="1"/>
+    <col min="8711" max="8960" width="8.83203125" style="8"/>
+    <col min="8961" max="8961" width="15.1640625" style="8" customWidth="1"/>
+    <col min="8962" max="8962" width="22.5" style="8" customWidth="1"/>
+    <col min="8963" max="8963" width="26.6640625" style="8" customWidth="1"/>
+    <col min="8964" max="8964" width="30.5" style="8" customWidth="1"/>
+    <col min="8965" max="8965" width="34" style="8" customWidth="1"/>
+    <col min="8966" max="8966" width="24.6640625" style="8" customWidth="1"/>
+    <col min="8967" max="9216" width="8.83203125" style="8"/>
+    <col min="9217" max="9217" width="15.1640625" style="8" customWidth="1"/>
+    <col min="9218" max="9218" width="22.5" style="8" customWidth="1"/>
+    <col min="9219" max="9219" width="26.6640625" style="8" customWidth="1"/>
+    <col min="9220" max="9220" width="30.5" style="8" customWidth="1"/>
+    <col min="9221" max="9221" width="34" style="8" customWidth="1"/>
+    <col min="9222" max="9222" width="24.6640625" style="8" customWidth="1"/>
+    <col min="9223" max="9472" width="8.83203125" style="8"/>
+    <col min="9473" max="9473" width="15.1640625" style="8" customWidth="1"/>
+    <col min="9474" max="9474" width="22.5" style="8" customWidth="1"/>
+    <col min="9475" max="9475" width="26.6640625" style="8" customWidth="1"/>
+    <col min="9476" max="9476" width="30.5" style="8" customWidth="1"/>
+    <col min="9477" max="9477" width="34" style="8" customWidth="1"/>
+    <col min="9478" max="9478" width="24.6640625" style="8" customWidth="1"/>
+    <col min="9479" max="9728" width="8.83203125" style="8"/>
+    <col min="9729" max="9729" width="15.1640625" style="8" customWidth="1"/>
+    <col min="9730" max="9730" width="22.5" style="8" customWidth="1"/>
+    <col min="9731" max="9731" width="26.6640625" style="8" customWidth="1"/>
+    <col min="9732" max="9732" width="30.5" style="8" customWidth="1"/>
+    <col min="9733" max="9733" width="34" style="8" customWidth="1"/>
+    <col min="9734" max="9734" width="24.6640625" style="8" customWidth="1"/>
+    <col min="9735" max="9984" width="8.83203125" style="8"/>
+    <col min="9985" max="9985" width="15.1640625" style="8" customWidth="1"/>
+    <col min="9986" max="9986" width="22.5" style="8" customWidth="1"/>
+    <col min="9987" max="9987" width="26.6640625" style="8" customWidth="1"/>
+    <col min="9988" max="9988" width="30.5" style="8" customWidth="1"/>
+    <col min="9989" max="9989" width="34" style="8" customWidth="1"/>
+    <col min="9990" max="9990" width="24.6640625" style="8" customWidth="1"/>
+    <col min="9991" max="10240" width="8.83203125" style="8"/>
+    <col min="10241" max="10241" width="15.1640625" style="8" customWidth="1"/>
+    <col min="10242" max="10242" width="22.5" style="8" customWidth="1"/>
+    <col min="10243" max="10243" width="26.6640625" style="8" customWidth="1"/>
+    <col min="10244" max="10244" width="30.5" style="8" customWidth="1"/>
+    <col min="10245" max="10245" width="34" style="8" customWidth="1"/>
+    <col min="10246" max="10246" width="24.6640625" style="8" customWidth="1"/>
+    <col min="10247" max="10496" width="8.83203125" style="8"/>
+    <col min="10497" max="10497" width="15.1640625" style="8" customWidth="1"/>
+    <col min="10498" max="10498" width="22.5" style="8" customWidth="1"/>
+    <col min="10499" max="10499" width="26.6640625" style="8" customWidth="1"/>
+    <col min="10500" max="10500" width="30.5" style="8" customWidth="1"/>
+    <col min="10501" max="10501" width="34" style="8" customWidth="1"/>
+    <col min="10502" max="10502" width="24.6640625" style="8" customWidth="1"/>
+    <col min="10503" max="10752" width="8.83203125" style="8"/>
+    <col min="10753" max="10753" width="15.1640625" style="8" customWidth="1"/>
+    <col min="10754" max="10754" width="22.5" style="8" customWidth="1"/>
+    <col min="10755" max="10755" width="26.6640625" style="8" customWidth="1"/>
+    <col min="10756" max="10756" width="30.5" style="8" customWidth="1"/>
+    <col min="10757" max="10757" width="34" style="8" customWidth="1"/>
+    <col min="10758" max="10758" width="24.6640625" style="8" customWidth="1"/>
+    <col min="10759" max="11008" width="8.83203125" style="8"/>
+    <col min="11009" max="11009" width="15.1640625" style="8" customWidth="1"/>
+    <col min="11010" max="11010" width="22.5" style="8" customWidth="1"/>
+    <col min="11011" max="11011" width="26.6640625" style="8" customWidth="1"/>
+    <col min="11012" max="11012" width="30.5" style="8" customWidth="1"/>
+    <col min="11013" max="11013" width="34" style="8" customWidth="1"/>
+    <col min="11014" max="11014" width="24.6640625" style="8" customWidth="1"/>
+    <col min="11015" max="11264" width="8.83203125" style="8"/>
+    <col min="11265" max="11265" width="15.1640625" style="8" customWidth="1"/>
+    <col min="11266" max="11266" width="22.5" style="8" customWidth="1"/>
+    <col min="11267" max="11267" width="26.6640625" style="8" customWidth="1"/>
+    <col min="11268" max="11268" width="30.5" style="8" customWidth="1"/>
+    <col min="11269" max="11269" width="34" style="8" customWidth="1"/>
+    <col min="11270" max="11270" width="24.6640625" style="8" customWidth="1"/>
+    <col min="11271" max="11520" width="8.83203125" style="8"/>
+    <col min="11521" max="11521" width="15.1640625" style="8" customWidth="1"/>
+    <col min="11522" max="11522" width="22.5" style="8" customWidth="1"/>
+    <col min="11523" max="11523" width="26.6640625" style="8" customWidth="1"/>
+    <col min="11524" max="11524" width="30.5" style="8" customWidth="1"/>
+    <col min="11525" max="11525" width="34" style="8" customWidth="1"/>
+    <col min="11526" max="11526" width="24.6640625" style="8" customWidth="1"/>
+    <col min="11527" max="11776" width="8.83203125" style="8"/>
+    <col min="11777" max="11777" width="15.1640625" style="8" customWidth="1"/>
+    <col min="11778" max="11778" width="22.5" style="8" customWidth="1"/>
+    <col min="11779" max="11779" width="26.6640625" style="8" customWidth="1"/>
+    <col min="11780" max="11780" width="30.5" style="8" customWidth="1"/>
+    <col min="11781" max="11781" width="34" style="8" customWidth="1"/>
+    <col min="11782" max="11782" width="24.6640625" style="8" customWidth="1"/>
+    <col min="11783" max="12032" width="8.83203125" style="8"/>
+    <col min="12033" max="12033" width="15.1640625" style="8" customWidth="1"/>
+    <col min="12034" max="12034" width="22.5" style="8" customWidth="1"/>
+    <col min="12035" max="12035" width="26.6640625" style="8" customWidth="1"/>
+    <col min="12036" max="12036" width="30.5" style="8" customWidth="1"/>
+    <col min="12037" max="12037" width="34" style="8" customWidth="1"/>
+    <col min="12038" max="12038" width="24.6640625" style="8" customWidth="1"/>
+    <col min="12039" max="12288" width="8.83203125" style="8"/>
+    <col min="12289" max="12289" width="15.1640625" style="8" customWidth="1"/>
+    <col min="12290" max="12290" width="22.5" style="8" customWidth="1"/>
+    <col min="12291" max="12291" width="26.6640625" style="8" customWidth="1"/>
+    <col min="12292" max="12292" width="30.5" style="8" customWidth="1"/>
+    <col min="12293" max="12293" width="34" style="8" customWidth="1"/>
+    <col min="12294" max="12294" width="24.6640625" style="8" customWidth="1"/>
+    <col min="12295" max="12544" width="8.83203125" style="8"/>
+    <col min="12545" max="12545" width="15.1640625" style="8" customWidth="1"/>
+    <col min="12546" max="12546" width="22.5" style="8" customWidth="1"/>
+    <col min="12547" max="12547" width="26.6640625" style="8" customWidth="1"/>
+    <col min="12548" max="12548" width="30.5" style="8" customWidth="1"/>
+    <col min="12549" max="12549" width="34" style="8" customWidth="1"/>
+    <col min="12550" max="12550" width="24.6640625" style="8" customWidth="1"/>
+    <col min="12551" max="12800" width="8.83203125" style="8"/>
+    <col min="12801" max="12801" width="15.1640625" style="8" customWidth="1"/>
+    <col min="12802" max="12802" width="22.5" style="8" customWidth="1"/>
+    <col min="12803" max="12803" width="26.6640625" style="8" customWidth="1"/>
+    <col min="12804" max="12804" width="30.5" style="8" customWidth="1"/>
+    <col min="12805" max="12805" width="34" style="8" customWidth="1"/>
+    <col min="12806" max="12806" width="24.6640625" style="8" customWidth="1"/>
+    <col min="12807" max="13056" width="8.83203125" style="8"/>
+    <col min="13057" max="13057" width="15.1640625" style="8" customWidth="1"/>
+    <col min="13058" max="13058" width="22.5" style="8" customWidth="1"/>
+    <col min="13059" max="13059" width="26.6640625" style="8" customWidth="1"/>
+    <col min="13060" max="13060" width="30.5" style="8" customWidth="1"/>
+    <col min="13061" max="13061" width="34" style="8" customWidth="1"/>
+    <col min="13062" max="13062" width="24.6640625" style="8" customWidth="1"/>
+    <col min="13063" max="13312" width="8.83203125" style="8"/>
+    <col min="13313" max="13313" width="15.1640625" style="8" customWidth="1"/>
+    <col min="13314" max="13314" width="22.5" style="8" customWidth="1"/>
+    <col min="13315" max="13315" width="26.6640625" style="8" customWidth="1"/>
+    <col min="13316" max="13316" width="30.5" style="8" customWidth="1"/>
+    <col min="13317" max="13317" width="34" style="8" customWidth="1"/>
+    <col min="13318" max="13318" width="24.6640625" style="8" customWidth="1"/>
+    <col min="13319" max="13568" width="8.83203125" style="8"/>
+    <col min="13569" max="13569" width="15.1640625" style="8" customWidth="1"/>
+    <col min="13570" max="13570" width="22.5" style="8" customWidth="1"/>
+    <col min="13571" max="13571" width="26.6640625" style="8" customWidth="1"/>
+    <col min="13572" max="13572" width="30.5" style="8" customWidth="1"/>
+    <col min="13573" max="13573" width="34" style="8" customWidth="1"/>
+    <col min="13574" max="13574" width="24.6640625" style="8" customWidth="1"/>
+    <col min="13575" max="13824" width="8.83203125" style="8"/>
+    <col min="13825" max="13825" width="15.1640625" style="8" customWidth="1"/>
+    <col min="13826" max="13826" width="22.5" style="8" customWidth="1"/>
+    <col min="13827" max="13827" width="26.6640625" style="8" customWidth="1"/>
+    <col min="13828" max="13828" width="30.5" style="8" customWidth="1"/>
+    <col min="13829" max="13829" width="34" style="8" customWidth="1"/>
+    <col min="13830" max="13830" width="24.6640625" style="8" customWidth="1"/>
+    <col min="13831" max="14080" width="8.83203125" style="8"/>
+    <col min="14081" max="14081" width="15.1640625" style="8" customWidth="1"/>
+    <col min="14082" max="14082" width="22.5" style="8" customWidth="1"/>
+    <col min="14083" max="14083" width="26.6640625" style="8" customWidth="1"/>
+    <col min="14084" max="14084" width="30.5" style="8" customWidth="1"/>
+    <col min="14085" max="14085" width="34" style="8" customWidth="1"/>
+    <col min="14086" max="14086" width="24.6640625" style="8" customWidth="1"/>
+    <col min="14087" max="14336" width="8.83203125" style="8"/>
+    <col min="14337" max="14337" width="15.1640625" style="8" customWidth="1"/>
+    <col min="14338" max="14338" width="22.5" style="8" customWidth="1"/>
+    <col min="14339" max="14339" width="26.6640625" style="8" customWidth="1"/>
+    <col min="14340" max="14340" width="30.5" style="8" customWidth="1"/>
+    <col min="14341" max="14341" width="34" style="8" customWidth="1"/>
+    <col min="14342" max="14342" width="24.6640625" style="8" customWidth="1"/>
+    <col min="14343" max="14592" width="8.83203125" style="8"/>
+    <col min="14593" max="14593" width="15.1640625" style="8" customWidth="1"/>
+    <col min="14594" max="14594" width="22.5" style="8" customWidth="1"/>
+    <col min="14595" max="14595" width="26.6640625" style="8" customWidth="1"/>
+    <col min="14596" max="14596" width="30.5" style="8" customWidth="1"/>
+    <col min="14597" max="14597" width="34" style="8" customWidth="1"/>
+    <col min="14598" max="14598" width="24.6640625" style="8" customWidth="1"/>
+    <col min="14599" max="14848" width="8.83203125" style="8"/>
+    <col min="14849" max="14849" width="15.1640625" style="8" customWidth="1"/>
+    <col min="14850" max="14850" width="22.5" style="8" customWidth="1"/>
+    <col min="14851" max="14851" width="26.6640625" style="8" customWidth="1"/>
+    <col min="14852" max="14852" width="30.5" style="8" customWidth="1"/>
+    <col min="14853" max="14853" width="34" style="8" customWidth="1"/>
+    <col min="14854" max="14854" width="24.6640625" style="8" customWidth="1"/>
+    <col min="14855" max="15104" width="8.83203125" style="8"/>
+    <col min="15105" max="15105" width="15.1640625" style="8" customWidth="1"/>
+    <col min="15106" max="15106" width="22.5" style="8" customWidth="1"/>
+    <col min="15107" max="15107" width="26.6640625" style="8" customWidth="1"/>
+    <col min="15108" max="15108" width="30.5" style="8" customWidth="1"/>
+    <col min="15109" max="15109" width="34" style="8" customWidth="1"/>
+    <col min="15110" max="15110" width="24.6640625" style="8" customWidth="1"/>
+    <col min="15111" max="15360" width="8.83203125" style="8"/>
+    <col min="15361" max="15361" width="15.1640625" style="8" customWidth="1"/>
+    <col min="15362" max="15362" width="22.5" style="8" customWidth="1"/>
+    <col min="15363" max="15363" width="26.6640625" style="8" customWidth="1"/>
+    <col min="15364" max="15364" width="30.5" style="8" customWidth="1"/>
+    <col min="15365" max="15365" width="34" style="8" customWidth="1"/>
+    <col min="15366" max="15366" width="24.6640625" style="8" customWidth="1"/>
+    <col min="15367" max="15616" width="8.83203125" style="8"/>
+    <col min="15617" max="15617" width="15.1640625" style="8" customWidth="1"/>
+    <col min="15618" max="15618" width="22.5" style="8" customWidth="1"/>
+    <col min="15619" max="15619" width="26.6640625" style="8" customWidth="1"/>
+    <col min="15620" max="15620" width="30.5" style="8" customWidth="1"/>
+    <col min="15621" max="15621" width="34" style="8" customWidth="1"/>
+    <col min="15622" max="15622" width="24.6640625" style="8" customWidth="1"/>
+    <col min="15623" max="15872" width="8.83203125" style="8"/>
+    <col min="15873" max="15873" width="15.1640625" style="8" customWidth="1"/>
+    <col min="15874" max="15874" width="22.5" style="8" customWidth="1"/>
+    <col min="15875" max="15875" width="26.6640625" style="8" customWidth="1"/>
+    <col min="15876" max="15876" width="30.5" style="8" customWidth="1"/>
+    <col min="15877" max="15877" width="34" style="8" customWidth="1"/>
+    <col min="15878" max="15878" width="24.6640625" style="8" customWidth="1"/>
+    <col min="15879" max="16128" width="8.83203125" style="8"/>
+    <col min="16129" max="16129" width="15.1640625" style="8" customWidth="1"/>
+    <col min="16130" max="16130" width="22.5" style="8" customWidth="1"/>
+    <col min="16131" max="16131" width="26.6640625" style="8" customWidth="1"/>
+    <col min="16132" max="16132" width="30.5" style="8" customWidth="1"/>
+    <col min="16133" max="16133" width="34" style="8" customWidth="1"/>
+    <col min="16134" max="16134" width="24.6640625" style="8" customWidth="1"/>
+    <col min="16135" max="16384" width="8.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:6" ht="18">
+      <c r="A1" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+    <row r="2" spans="1:6" s="12" customFormat="1">
+      <c r="A2" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="16">
+    <row r="3" spans="1:6" ht="28">
+      <c r="A3" s="13">
         <v>42296</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
+    <row r="4" spans="1:6" ht="70">
+      <c r="A4" s="13">
         <v>42297</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="8" t="s">
         <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="B5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>